<commit_message>
add new exercises, fix answer, words, etc.
- updated dictionary definitions.
- fixed kanji not being accepted in an answer for lesson-9/workbook-2; 嫌い can be used now.
- added missing words to lesson-12/vocab-7; 目医者 and 歯医者. Decks/wordlists have been updated with these. (#145)
- added the following exercises.

# Lesson 22 (3rd ed.)
- Kanji Practice: Write the Readings
</commit_message>
<xml_diff>
--- a/resources/tools/wordlist_E-J/lessons-3rd/lesson-12.xlsx
+++ b/resources/tools/wordlist_E-J/lessons-3rd/lesson-12.xlsx
@@ -1329,7 +1329,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>眼科|がんか</t>
+          <t>眼科／目医者|がんか／めいしゃ</t>
         </is>
       </c>
     </row>
@@ -1341,7 +1341,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>歯科|しか</t>
+          <t>歯科／歯医者|しか／はいしゃ</t>
         </is>
       </c>
     </row>

</xml_diff>